<commit_message>
Scripts prontos/ Inicio da ducumentação
</commit_message>
<xml_diff>
--- a/sprint1-bd-spmedgroup/Modelagem/SpMedicGroup_Fisico.xlsx
+++ b/sprint1-bd-spmedgroup/Modelagem/SpMedicGroup_Fisico.xlsx
@@ -1,39 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\Desktop\senai\sprint1-bd\sprint1-bd-spmedgroup\Modelagem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43442346851\Desktop\sprint1-bd\sprint1-bd-spmedgroup\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F386F539-6977-4AFB-91D2-93113E74A23A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA40DD57-5289-43F5-A669-ED0FF70C6F5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{480B0941-BFCA-4E68-990C-C4800C207D19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{480B0941-BFCA-4E68-990C-C4800C207D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>TipoUsuario</t>
   </si>
@@ -116,30 +109,6 @@
     <t>Senha</t>
   </si>
   <si>
-    <t>adm@adm.com</t>
-  </si>
-  <si>
-    <t>adm123</t>
-  </si>
-  <si>
-    <t>Carol</t>
-  </si>
-  <si>
-    <t>carol@email.com</t>
-  </si>
-  <si>
-    <t>carol123</t>
-  </si>
-  <si>
-    <t>Saulo</t>
-  </si>
-  <si>
-    <t>saulo@email.com</t>
-  </si>
-  <si>
-    <t>saulo123</t>
-  </si>
-  <si>
     <t>Nome</t>
   </si>
   <si>
@@ -207,6 +176,57 @@
   </si>
   <si>
     <t>DataConsulta</t>
+  </si>
+  <si>
+    <t>NomeFantasia</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>cadu12@gmail.com</t>
+  </si>
+  <si>
+    <t>adm@gmail.com</t>
+  </si>
+  <si>
+    <t>adm1243</t>
+  </si>
+  <si>
+    <t>cadu1243</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>nico1243</t>
+  </si>
+  <si>
+    <t>Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200 </t>
+  </si>
+  <si>
+    <t>nico12@gmail.com</t>
+  </si>
+  <si>
+    <t>ana12@gmail.com</t>
+  </si>
+  <si>
+    <t>ana1243</t>
+  </si>
+  <si>
+    <t>53536t5656</t>
+  </si>
+  <si>
+    <t>Ana Laura</t>
+  </si>
+  <si>
+    <t>Dor na garganta</t>
+  </si>
+  <si>
+    <t>2903/SP</t>
   </si>
 </sst>
 </file>
@@ -349,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,52 +390,58 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -733,47 +759,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0DB8F4-6389-42CA-812C-A2417FC7ED67}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="32.85546875" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
+    <col min="9" max="9" width="32.88671875" customWidth="1"/>
+    <col min="10" max="10" width="48.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="23"/>
+      <c r="D1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="G1" s="10" t="s">
+      <c r="E1" s="22"/>
+      <c r="G1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -790,7 +816,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>16</v>
@@ -802,7 +828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -831,7 +857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -845,7 +871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -859,233 +885,266 @@
         <v>11</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="7"/>
       <c r="D6" s="4">
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D7" s="4">
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="22">
-        <v>1</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="17">
+        <v>1</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="22">
+      <c r="G8" s="17">
         <v>2</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G9" s="17">
+        <v>3</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>1</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G9" s="22">
+      <c r="E13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="15">
+        <v>33092</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="13">
+        <v>637438537</v>
+      </c>
+      <c r="I13" s="13">
+        <v>3798378967893</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>2</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="15">
+        <v>37709</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="13">
+        <v>78373748</v>
+      </c>
+      <c r="I14" s="13">
+        <v>789878997839</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
         <v>3</v>
       </c>
-      <c r="H9" s="22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
-        <v>1</v>
-      </c>
-      <c r="B13" s="15">
-        <v>1</v>
-      </c>
-      <c r="C13" s="15" t="s">
+      <c r="B15" s="11">
         <v>3</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="19">
-        <v>33092</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="17">
-        <v>637438537</v>
-      </c>
-      <c r="I13" s="17">
-        <v>3798378967893</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <v>2</v>
-      </c>
-      <c r="B14" s="15">
-        <v>2</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="19">
-        <v>32964</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="17">
-        <v>78373748</v>
-      </c>
-      <c r="I14" s="17">
-        <v>789878997839</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="C15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="15">
+        <v>37846</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="13">
+        <v>378738937889</v>
+      </c>
+      <c r="I15" s="13">
+        <v>39789878979</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>4</v>
+      </c>
+      <c r="B16" s="13">
         <v>3</v>
       </c>
-      <c r="B15" s="15">
-        <v>3</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="15" t="s">
+      <c r="C16" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="25">
+        <v>37112</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="13">
+        <v>434243243534</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>34</v>
-      </c>
-      <c r="F15" s="19">
-        <v>32996</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="17">
-        <v>378738937889</v>
-      </c>
-      <c r="I15" s="17">
-        <v>39789878979</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>42</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
-      <c r="E17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="21" t="s">
+      <c r="E17" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>44</v>
+      <c r="C18" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>7</v>
@@ -1097,18 +1156,18 @@
         <v>24</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
-        <v>1</v>
-      </c>
-      <c r="B19" s="22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="17">
+        <v>1</v>
+      </c>
+      <c r="B19" s="17">
         <v>3</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>45</v>
+      <c r="C19" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="E19" s="6">
         <v>1</v>
@@ -1122,37 +1181,48 @@
       <c r="H19" s="6">
         <v>2</v>
       </c>
-      <c r="I19" s="6">
-        <v>5141985</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="17">
+        <v>2</v>
+      </c>
+      <c r="B20" s="17">
+        <v>4</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
         <v>1</v>
       </c>
@@ -1165,27 +1235,57 @@
       <c r="E24" s="4">
         <v>1</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="18">
+        <v>43890.583333333336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="4">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="18">
         <v>43890.583333333336</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="E17:I17"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1" xr:uid="{806E2792-E957-49A7-9E41-9C600923FCA6}"/>
     <hyperlink ref="D14" r:id="rId2" xr:uid="{BECBF57A-4825-491E-B6DB-DCFC489FDB77}"/>
     <hyperlink ref="D15" r:id="rId3" xr:uid="{E69C19BD-27B0-4A8E-A8BF-CC65AC650779}"/>
+    <hyperlink ref="D16" r:id="rId4" xr:uid="{9E190D0C-AB4A-4D9D-841D-227E7D51C392}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD9E788-46FC-4CE8-95B9-1BAD9E8890DD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>